<commit_message>
Se agrega database de perfiles canal | Pequeñas correcciones a la definicion de clases
</commit_message>
<xml_diff>
--- a/database/Tabla_CANAL.xlsx
+++ b/database/Tabla_CANAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiez\Documents\cirsoc301\cirsoc301\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Documents\cirsoc301\cirsoc301\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B9D03A-618F-4EF7-8630-817D3D65ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB8BFEF-A8F6-4E22-A1F5-BA402C34684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA" sheetId="1" r:id="rId1"/>
@@ -3213,14 +3213,14 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="32" max="32" width="11.5703125" customWidth="1"/>
+    <col min="32" max="32" width="26.85546875" customWidth="1"/>
     <col min="33" max="33" width="12.7109375" customWidth="1"/>
     <col min="34" max="34" width="15.5703125" customWidth="1"/>
   </cols>

</xml_diff>